<commit_message>
added high temperature heat pump inventory form literature
</commit_message>
<xml_diff>
--- a/inventories/lci-EP2050.xlsx
+++ b/inventories/lci-EP2050.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="219">
   <si>
     <t xml:space="preserve">cutoff</t>
   </si>
@@ -83,6 +83,117 @@
   </si>
   <si>
     <t xml:space="preserve">production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heat from high temperature heat pump, 250 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleup of 10kW pump from https://doi.org/10.1016/j.spc.2023.06.016 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethane, 1,1,1,2-tetrafluoro-, HFC-134a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kilogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">air::urban air close to ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cubic meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water, unspecified natural origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natural resource::in water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for copper, cathode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">technosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copper, cathode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for electricity, medium voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kilowatt hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity, medium voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for heat, district or industrial, natural gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heat, district or industrial, natural gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for lubricating oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lubricating oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for polyvinylchloride, bulk polymerised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">polyvinylchloride, bulk polymerised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for refrigerant R134a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refrigerant R134a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for reinforcing steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reinforcing steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for steel, low-alloyed, hot rolled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steel, low-alloyed, hot rolled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for tube insulation, elastomere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tube insulation, elastomere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">market for waste plastic, mixture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waste plastic, mixture</t>
   </si>
   <si>
     <t xml:space="preserve">hydrogen production, gaseous, 30 bar, from PEM electrolysis, from grid electricity, domestic, EP2050</t>
@@ -95,21 +206,9 @@
     <t xml:space="preserve">hydrogen, gaseous, 30 bar</t>
   </si>
   <si>
-    <t xml:space="preserve">CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kilogram</t>
-  </si>
-  <si>
     <t xml:space="preserve">electrolyzer production, 1MWe, PEM, Stack</t>
   </si>
   <si>
-    <t xml:space="preserve">RER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">technosphere</t>
-  </si>
-  <si>
     <t xml:space="preserve">electrolyzer, 1MWe, PEM, Stack</t>
   </si>
   <si>
@@ -146,9 +245,6 @@
     <t xml:space="preserve">market for electricity, low voltage</t>
   </si>
   <si>
-    <t xml:space="preserve">kilowatt hour</t>
-  </si>
-  <si>
     <t xml:space="preserve">electricity, low voltage</t>
   </si>
   <si>
@@ -170,12 +266,6 @@
     <t xml:space="preserve">Oxygen</t>
   </si>
   <si>
-    <t xml:space="preserve">air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biosphere</t>
-  </si>
-  <si>
     <t xml:space="preserve">Occupation, unspecified</t>
   </si>
   <si>
@@ -224,9 +314,6 @@
     <t xml:space="preserve">Gas-to-liquid plant construction</t>
   </si>
   <si>
-    <t xml:space="preserve">GLO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gas-to-liquid plant</t>
   </si>
   <si>
@@ -320,18 +407,12 @@
     <t xml:space="preserve">market group for electricity, medium voltage</t>
   </si>
   <si>
-    <t xml:space="preserve">electricity, medium voltage</t>
-  </si>
-  <si>
     <t xml:space="preserve">of which 0.078kWh to compress CO2 from 1 atm to 25 bar</t>
   </si>
   <si>
     <t xml:space="preserve">heat production, natural gas, at industrial furnace &gt;100kW</t>
   </si>
   <si>
-    <t xml:space="preserve">heat, district or industrial, natural gas</t>
-  </si>
-  <si>
     <t xml:space="preserve">carbon dioxide compression, transport and storage</t>
   </si>
   <si>
@@ -344,9 +425,6 @@
     <t xml:space="preserve">Carbon dioxide, non-fossil</t>
   </si>
   <si>
-    <t xml:space="preserve">air::urban air close to ground</t>
-  </si>
-  <si>
     <t xml:space="preserve">pipeline of 1 km long</t>
   </si>
   <si>
@@ -384,9 +462,6 @@
   </si>
   <si>
     <t xml:space="preserve">market for rainwater mineral oil storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cubic meter</t>
   </si>
   <si>
     <t xml:space="preserve">rainwater mineral oil storage</t>
@@ -522,9 +597,6 @@
   </si>
   <si>
     <t xml:space="preserve">methane, from electrochemical methanation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">market for electricity, medium voltage</t>
   </si>
   <si>
     <t xml:space="preserve">market for heat, central or small-scale, biomethane</t>
@@ -718,12 +790,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -745,13 +817,14 @@
   </sheetPr>
   <dimension ref="A1:L311"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,30 +1000,425 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="str">
+        <f aca="false">B17</f>
+        <v>heat from high temperature heat pump, 250 kW</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f aca="false">B18</f>
+        <v>GLO</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f aca="false">B22</f>
+        <v>megajoule</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0.1062</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.6018</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.708</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>521</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>3315</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>3150</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1776</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>474</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>237</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <f aca="false">-B39-B35</f>
+        <v>-261</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -962,14 +1430,14 @@
         <v>3</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="4" t="n">
+      <c r="B50" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -977,8 +1445,8 @@
       <c r="A51" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>22</v>
+      <c r="B51" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,7 +1454,7 @@
         <v>8</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,7 +1462,7 @@
         <v>5</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,13 +1506,13 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" s="4" t="n">
+        <v>58</v>
+      </c>
+      <c r="B57" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>25</v>
@@ -1053,179 +1521,179 @@
         <v>20</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="4" t="n">
+        <v>61</v>
+      </c>
+      <c r="B58" s="5" t="n">
         <v>1.35E-006</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="B59" s="5" t="n">
         <v>3.37E-007</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B60" s="4" t="n">
+        <v>67</v>
+      </c>
+      <c r="B60" s="5" t="n">
         <v>-1.35E-006</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B61" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="B61" s="5" t="n">
         <v>-3.37E-007</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B62" s="4" t="n">
+        <v>73</v>
+      </c>
+      <c r="B62" s="5" t="n">
         <v>54</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B63" s="4" t="n">
+        <v>76</v>
+      </c>
+      <c r="B63" s="5" t="n">
         <v>14</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B64" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="B64" s="5" t="n">
         <v>8</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B65" s="4" t="n">
+        <v>81</v>
+      </c>
+      <c r="B65" s="5" t="n">
         <v>0.000607</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,14 +1701,14 @@
         <v>3</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B68" s="4" t="n">
+      <c r="B68" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1248,8 +1716,8 @@
       <c r="A69" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>22</v>
+      <c r="B69" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,7 +1725,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,7 +1733,7 @@
         <v>5</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1309,13 +1777,13 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B75" s="4" t="n">
+        <v>84</v>
+      </c>
+      <c r="B75" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>25</v>
@@ -1324,179 +1792,179 @@
         <v>20</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="4" t="n">
+        <v>61</v>
+      </c>
+      <c r="B76" s="5" t="n">
         <v>1.35E-006</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B77" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="B77" s="5" t="n">
         <v>3.37E-007</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B78" s="4" t="n">
+        <v>67</v>
+      </c>
+      <c r="B78" s="5" t="n">
         <v>-1.35E-006</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B79" s="4" t="n">
+        <v>70</v>
+      </c>
+      <c r="B79" s="5" t="n">
         <v>-3.37E-007</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B80" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="B80" s="5" t="n">
         <v>54</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B81" s="4" t="n">
+        <v>76</v>
+      </c>
+      <c r="B81" s="5" t="n">
         <v>14</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B82" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" s="5" t="n">
         <v>8</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B83" s="4" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" s="5" t="n">
         <v>0.000607</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,7 +1972,7 @@
         <v>3</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,7 +1988,7 @@
         <v>8</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1544,7 +2012,7 @@
         <v>5</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,15 +2020,15 @@
         <v>14</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,7 +2059,7 @@
         <v>8</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="I94" s="0" t="s">
         <v>14</v>
@@ -1599,13 +2067,13 @@
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>25</v>
@@ -1614,64 +2082,64 @@
         <v>20</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="H95" s="0" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="I95" s="0" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>2.26</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="H96" s="0" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B97" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="5" t="n">
         <v>6.7E-012</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="H97" s="0" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>0.05</v>
@@ -1680,13 +2148,13 @@
         <v>25</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H98" s="0" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,7 +2162,7 @@
         <v>3</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,7 +2178,7 @@
         <v>8</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,7 +2202,7 @@
         <v>5</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,15 +2210,15 @@
         <v>14</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,53 +2251,53 @@
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>0.875</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>0.125</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D112" s="0" t="s">
         <v>25</v>
@@ -1838,24 +2306,24 @@
         <v>20</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>5.71E-006</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F113" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +2331,7 @@
         <v>3</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,7 +2347,7 @@
         <v>8</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,7 +2379,7 @@
         <v>14</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,13 +2412,13 @@
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D124" s="0" t="s">
         <v>25</v>
@@ -1959,67 +2427,67 @@
         <v>20</v>
       </c>
       <c r="G124" s="0" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>0.07</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F125" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>1.57</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F126" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G126" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B127" s="4" t="n">
+        <v>111</v>
+      </c>
+      <c r="B127" s="5" t="n">
         <v>1.93E-009</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2027,7 +2495,7 @@
         <v>3</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,7 +2503,7 @@
         <v>5</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,7 +2519,7 @@
         <v>8</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,15 +2527,15 @@
         <v>14</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,13 +2571,13 @@
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D137" s="0" t="s">
         <v>25</v>
@@ -2118,184 +2586,184 @@
         <v>20</v>
       </c>
       <c r="G137" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B138" s="4" t="n">
+        <v>116</v>
+      </c>
+      <c r="B138" s="5" t="n">
         <v>5E-011</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D138" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F138" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G138" s="0" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B139" s="4" t="n">
+        <v>118</v>
+      </c>
+      <c r="B139" s="5" t="n">
         <v>-5E-011</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D139" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F139" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G139" s="0" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>3.437</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D140" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F140" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G140" s="0" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>0.004</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D141" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F141" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G141" s="0" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="H141" s="0" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>0.0035</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D142" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F142" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G142" s="0" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="H142" s="0" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>0.345</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F143" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G143" s="0" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="H143" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>6.28</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D144" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F144" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G144" s="0" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D145" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F145" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G145" s="0" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="H145" s="0" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>1</v>
@@ -2304,30 +2772,30 @@
         <v>25</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="F146" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B147" s="4" t="n">
+        <v>133</v>
+      </c>
+      <c r="B147" s="5" t="n">
         <v>0.021</v>
       </c>
       <c r="D147" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="F147" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H147" s="0" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2335,7 +2803,7 @@
         <v>3</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,7 +2811,7 @@
         <v>5</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,7 +2827,7 @@
         <v>8</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2408,13 +2876,13 @@
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D157" s="0" t="s">
         <v>25</v>
@@ -2423,232 +2891,232 @@
         <v>20</v>
       </c>
       <c r="G157" s="0" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>1.00057</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D158" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F158" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G158" s="0" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>0.0067</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F159" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G159" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>-0.000168</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D160" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F160" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G160" s="0" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>0.000584</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D161" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F161" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G161" s="0" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B162" s="4" t="n">
+        <v>142</v>
+      </c>
+      <c r="B162" s="5" t="n">
         <v>2.6E-010</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D162" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F162" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G162" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>-6.27E-006</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D163" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F163" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G163" s="0" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>-7.5E-005</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
       <c r="F164" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G164" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>0.000689</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D165" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F165" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G165" s="0" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>0.0336</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="F166" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G166" s="0" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>0.0326</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="F167" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G167" s="0" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>-6.89E-007</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
       <c r="F168" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G168" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>0.0017898</v>
@@ -2657,10 +3125,10 @@
         <v>25</v>
       </c>
       <c r="E169" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F169" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2668,7 +3136,7 @@
         <v>3</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,7 +3152,7 @@
         <v>14</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2692,7 +3160,7 @@
         <v>8</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2713,10 +3181,10 @@
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,23 +3192,23 @@
         <v>5</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B179" s="5" t="s">
-        <v>134</v>
+      <c r="B179" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2771,41 +3239,41 @@
         <v>8</v>
       </c>
       <c r="H182" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D183" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F183" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G183" s="0" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="H183" s="0" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D184" s="0" t="s">
         <v>25</v>
@@ -2814,35 +3282,35 @@
         <v>20</v>
       </c>
       <c r="G184" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="H184" s="0" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>0.336206897</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F185" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G185" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>0.132067588</v>
@@ -2851,56 +3319,56 @@
         <v>25</v>
       </c>
       <c r="E186" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F186" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H186" s="0" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B187" s="4" t="n">
+        <v>164</v>
+      </c>
+      <c r="B187" s="5" t="n">
         <v>1.67E-006</v>
       </c>
       <c r="D187" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E187" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F187" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H187" s="0" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>12.45682789</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F188" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G188" s="0" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="H188" s="0" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,7 +3376,7 @@
         <v>3</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,7 +3392,7 @@
         <v>8</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,23 +3416,23 @@
         <v>5</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B196" s="5" t="s">
-        <v>141</v>
+      <c r="B196" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2997,33 +3465,33 @@
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>12.89</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D200" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F200" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G200" s="0" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="B201" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D201" s="0" t="s">
         <v>25</v>
@@ -3032,167 +3500,167 @@
         <v>20</v>
       </c>
       <c r="G201" s="0" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B202" s="0" t="n">
         <v>68.81959911</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D202" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F202" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G202" s="0" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B203" s="0" t="n">
         <v>0.302895323</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F203" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G203" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B204" s="4" t="n">
+        <v>167</v>
+      </c>
+      <c r="B204" s="5" t="n">
         <v>7.93E-006</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F204" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G204" s="0" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B205" s="4" t="n">
+        <v>169</v>
+      </c>
+      <c r="B205" s="5" t="n">
         <v>2.11E-005</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F205" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G205" s="0" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B206" s="4" t="n">
+        <v>171</v>
+      </c>
+      <c r="B206" s="5" t="n">
         <v>3.96E-006</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F206" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G206" s="0" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B207" s="0" t="n">
         <v>0.138975501</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F207" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G207" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B208" s="0" t="n">
         <v>1.690423163</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D208" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F208" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G208" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="B209" s="0" t="n">
         <v>-0.068819599</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
       <c r="F209" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G209" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3200,7 +3668,7 @@
         <v>3</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3216,7 +3684,7 @@
         <v>8</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3240,7 +3708,7 @@
         <v>5</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3248,15 +3716,15 @@
         <v>14</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3284,7 +3752,7 @@
         <v>10</v>
       </c>
       <c r="G220" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="H220" s="0" t="s">
         <v>8</v>
@@ -3295,13 +3763,13 @@
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="B221" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D221" s="0" t="s">
         <v>25</v>
@@ -3310,38 +3778,38 @@
         <v>20</v>
       </c>
       <c r="G221" s="0" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="H221" s="0" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>2.371</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D222" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F222" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G222" s="0" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="H222" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>0.11</v>
@@ -3350,65 +3818,65 @@
         <v>25</v>
       </c>
       <c r="E223" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F223" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="G223" s="0" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="I223" s="0" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B224" s="0" t="n">
         <v>0.0436264</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F224" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G224" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="H224" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B225" s="0" t="n">
         <v>0.02371</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F225" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G225" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="H225" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="I225" s="0" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,7 +3884,7 @@
         <v>3</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3424,7 +3892,7 @@
         <v>5</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3440,7 +3908,7 @@
         <v>8</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3489,13 +3957,13 @@
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="B235" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C235" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D235" s="0" t="s">
         <v>25</v>
@@ -3504,232 +3972,232 @@
         <v>20</v>
       </c>
       <c r="G235" s="0" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="B236" s="0" t="n">
         <v>1.00057</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D236" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F236" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G236" s="0" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>0.0067</v>
       </c>
       <c r="C237" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D237" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F237" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G237" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>-0.000168</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D238" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F238" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G238" s="0" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>0.000584</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D239" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F239" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G239" s="0" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B240" s="4" t="n">
+        <v>142</v>
+      </c>
+      <c r="B240" s="5" t="n">
         <v>2.6E-010</v>
       </c>
       <c r="C240" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D240" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F240" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G240" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>-6.27E-006</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D241" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F241" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G241" s="0" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>-7.5E-005</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D242" s="0" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
       <c r="F242" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G242" s="0" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>0.000689</v>
       </c>
       <c r="C243" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D243" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F243" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G243" s="0" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>0.0336</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D244" s="0" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="F244" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G244" s="0" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>0.0326</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D245" s="0" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="F245" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G245" s="0" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>-6.89E-007</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D246" s="0" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
       <c r="F246" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G246" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>0.0017898</v>
@@ -3738,10 +4206,10 @@
         <v>25</v>
       </c>
       <c r="E247" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F247" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3749,7 +4217,7 @@
         <v>3</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3757,7 +4225,7 @@
         <v>5</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,7 +4241,7 @@
         <v>8</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3797,15 +4265,15 @@
         <v>14</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B256" s="0" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3821,7 +4289,7 @@
         <v>18</v>
       </c>
       <c r="C258" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D258" s="0" t="s">
         <v>5</v>
@@ -3841,16 +4309,16 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="B259" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C259" s="0" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="D259" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F259" s="0" t="s">
         <v>25</v>
@@ -3859,202 +4327,202 @@
         <v>20</v>
       </c>
       <c r="H259" s="0" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="B260" s="0" t="n">
         <v>1.02</v>
       </c>
       <c r="C260" s="0" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="D260" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F260" s="0" t="s">
         <v>25</v>
       </c>
       <c r="G260" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H260" s="0" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="B261" s="0" t="n">
         <v>0.209888988</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D261" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F261" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G261" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H261" s="0" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="B262" s="0" t="n">
         <v>0.041393706</v>
       </c>
       <c r="C262" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D262" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F262" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G262" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H262" s="0" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="B263" s="4" t="n">
+        <v>193</v>
+      </c>
+      <c r="B263" s="5" t="n">
         <v>2.34E-008</v>
       </c>
       <c r="C263" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D263" s="0" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="F263" s="0" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="G263" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H263" s="0" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B264" s="4" t="n">
+        <v>197</v>
+      </c>
+      <c r="B264" s="5" t="n">
         <v>8.48E-008</v>
       </c>
       <c r="C264" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D264" s="0" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="F264" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G264" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H264" s="0" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B265" s="4" t="n">
+        <v>133</v>
+      </c>
+      <c r="B265" s="5" t="n">
         <v>1.39E-005</v>
       </c>
       <c r="C265" s="0" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="E265" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F265" s="0" t="s">
         <v>25</v>
       </c>
       <c r="G265" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="B266" s="4" t="n">
+        <v>199</v>
+      </c>
+      <c r="B266" s="5" t="n">
         <v>4.4E-009</v>
       </c>
       <c r="C266" s="0" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="E266" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F266" s="0" t="s">
         <v>25</v>
       </c>
       <c r="G266" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B267" s="0" t="n">
         <v>0.00030042</v>
       </c>
       <c r="C267" s="0" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="E267" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F267" s="0" t="s">
         <v>25</v>
       </c>
       <c r="G267" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="B268" s="4" t="n">
+        <v>201</v>
+      </c>
+      <c r="B268" s="5" t="n">
         <v>1.2E-006</v>
       </c>
       <c r="C268" s="0" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="E268" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F268" s="0" t="s">
         <v>25</v>
       </c>
       <c r="G268" s="0" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4062,7 +4530,7 @@
         <v>3</v>
       </c>
       <c r="B270" s="0" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4078,7 +4546,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="0" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4102,7 +4570,7 @@
         <v>5</v>
       </c>
       <c r="B275" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4110,15 +4578,15 @@
         <v>14</v>
       </c>
       <c r="B276" s="0" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B277" s="0" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4146,16 +4614,16 @@
         <v>10</v>
       </c>
       <c r="G279" s="0" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="H279" s="0" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="I279" s="0" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="J279" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="K279" s="0" t="s">
         <v>8</v>
@@ -4166,48 +4634,48 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="B280" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C280" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D280" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E280" s="0" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="F280" s="0" t="s">
         <v>20</v>
       </c>
       <c r="J280" s="0" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="K280" s="0" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B281" s="4" t="n">
+        <v>207</v>
+      </c>
+      <c r="B281" s="5" t="n">
         <v>8.06E-006</v>
       </c>
       <c r="C281" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D281" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E281" s="0" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="F281" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G281" s="0" t="n">
         <v>2</v>
@@ -4219,30 +4687,30 @@
         <v>0.418623762</v>
       </c>
       <c r="J281" s="0" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="K281" s="0" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B282" s="0" t="n">
         <v>2.768361582</v>
       </c>
       <c r="C282" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D282" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E282" s="0" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="F282" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G282" s="0" t="n">
         <v>2</v>
@@ -4254,59 +4722,59 @@
         <v>0.206054825</v>
       </c>
       <c r="J282" s="0" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="K282" s="0" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B283" s="0" t="n">
         <v>0.50779661</v>
       </c>
       <c r="C283" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D283" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E283" s="0" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="F283" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G283" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J283" s="0" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="K283" s="0" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="B284" s="0" t="n">
         <v>0.000176554</v>
       </c>
       <c r="C284" s="0" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D284" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E284" s="0" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="F284" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G284" s="0" t="n">
         <v>2</v>
@@ -4318,10 +4786,10 @@
         <v>0.074210003</v>
       </c>
       <c r="J284" s="0" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="K284" s="0" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4329,7 +4797,7 @@
         <v>3</v>
       </c>
       <c r="B286" s="0" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4337,7 +4805,7 @@
         <v>5</v>
       </c>
       <c r="B287" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4353,7 +4821,7 @@
         <v>8</v>
       </c>
       <c r="B289" s="0" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4377,15 +4845,15 @@
         <v>14</v>
       </c>
       <c r="B292" s="0" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B293" s="0" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4401,7 +4869,7 @@
         <v>18</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D295" s="0" t="s">
         <v>5</v>
@@ -4421,16 +4889,16 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="B296" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F296" s="0" t="s">
         <v>25</v>
@@ -4439,53 +4907,53 @@
         <v>20</v>
       </c>
       <c r="H296" s="0" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>0.09375</v>
       </c>
       <c r="C297" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D297" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F297" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G297" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H297" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B298" s="0" t="n">
         <v>31.25</v>
       </c>
       <c r="C298" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D298" s="0" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="F298" s="0" t="s">
         <v>25</v>
       </c>
       <c r="G298" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H298" s="0" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4493,7 +4961,7 @@
         <v>3</v>
       </c>
       <c r="B300" s="0" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4501,7 +4969,7 @@
         <v>5</v>
       </c>
       <c r="B301" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,7 +4985,7 @@
         <v>8</v>
       </c>
       <c r="B303" s="0" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4540,16 +5008,16 @@
       <c r="A306" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B306" s="5" t="s">
-        <v>194</v>
+      <c r="B306" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B307" s="0" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4565,7 +5033,7 @@
         <v>18</v>
       </c>
       <c r="C309" s="0" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="D309" s="0" t="s">
         <v>5</v>
@@ -4585,16 +5053,16 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="B310" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C310" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D310" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F310" s="0" t="s">
         <v>25</v>
@@ -4603,30 +5071,30 @@
         <v>20</v>
       </c>
       <c r="H310" s="0" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B311" s="0" t="n">
         <v>0.344</v>
       </c>
       <c r="C311" s="0" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F311" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G311" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H311" s="0" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>